<commit_message>
new test dataset and associated processing
</commit_message>
<xml_diff>
--- a/models/2024-5-31-models_7/results.xlsx
+++ b/models/2024-5-31-models_7/results.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="20_ISIC_DiDI" sheetId="1" r:id="rId1"/>
+    <sheet name="20-ISIC-DiDI" sheetId="1" r:id="rId1"/>
     <sheet name="ISIC_DiDI" sheetId="2" r:id="rId2"/>
     <sheet name="DiDI" sheetId="3" r:id="rId3"/>
     <sheet name="BrAD" sheetId="4" r:id="rId4"/>
+    <sheet name="REZK" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>accuracy</t>
   </si>
@@ -423,22 +424,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8274739583333334</v>
+        <v>0.82890625</v>
       </c>
       <c r="C2">
-        <v>0.8871297933406891</v>
+        <v>0.8902795167807954</v>
       </c>
       <c r="D2">
-        <v>0.7842065856931557</v>
+        <v>0.7857095047591347</v>
       </c>
       <c r="E2">
-        <v>0.90390625</v>
+        <v>0.9067708333333333</v>
       </c>
       <c r="F2">
-        <v>0.7842065856931557</v>
+        <v>0.7857095047591347</v>
       </c>
       <c r="G2">
-        <v>0.8396705186447477</v>
+        <v>0.8414532847882495</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -446,22 +447,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.951953125</v>
+        <v>0.9567708333333333</v>
       </c>
       <c r="C3">
-        <v>0.9890506609699876</v>
+        <v>0.9922172464298219</v>
       </c>
       <c r="D3">
-        <v>0.9201869125083912</v>
+        <v>0.9266042355580453</v>
       </c>
       <c r="E3">
-        <v>0.98984375</v>
+        <v>0.9927083333333333</v>
       </c>
       <c r="F3">
-        <v>0.9201869125083912</v>
+        <v>0.9266042355580453</v>
       </c>
       <c r="G3">
-        <v>0.9537189618486555</v>
+        <v>0.9583827962286656</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -469,22 +470,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.8583333333333333</v>
+        <v>0.8580729166666666</v>
       </c>
       <c r="C4">
-        <v>0.9831868877242285</v>
+        <v>0.9833634990528149</v>
       </c>
       <c r="D4">
-        <v>0.7849175899067331</v>
+        <v>0.7851087919200189</v>
       </c>
       <c r="E4">
         <v>0.9875</v>
       </c>
       <c r="F4">
-        <v>0.7849175899067331</v>
+        <v>0.7851087919200189</v>
       </c>
       <c r="G4">
-        <v>0.8745856172086931</v>
+        <v>0.8745400347457845</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -492,22 +493,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.8415364583333333</v>
+        <v>0.8450520833333334</v>
       </c>
       <c r="C5">
-        <v>0.9148121630267977</v>
+        <v>0.92221541952537</v>
       </c>
       <c r="D5">
-        <v>0.790564177630348</v>
+        <v>0.7928836980892566</v>
       </c>
       <c r="E5">
-        <v>0.9294270833333333</v>
+        <v>0.9354166666666667</v>
       </c>
       <c r="F5">
-        <v>0.790564177630348</v>
+        <v>0.7928836980892566</v>
       </c>
       <c r="G5">
-        <v>0.8542995004591324</v>
+        <v>0.8579287640738509</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -515,22 +516,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.9526041666666667</v>
+        <v>0.9502604166666667</v>
       </c>
       <c r="C6">
-        <v>0.9918468409438118</v>
+        <v>0.9932736999445972</v>
       </c>
       <c r="D6">
-        <v>0.9192835589197403</v>
+        <v>0.9147769671847101</v>
       </c>
       <c r="E6">
-        <v>0.9924479166666667</v>
+        <v>0.99375</v>
       </c>
       <c r="F6">
-        <v>0.9192835589197403</v>
+        <v>0.9147769671847101</v>
       </c>
       <c r="G6">
-        <v>0.9544333556268998</v>
+        <v>0.9524653153464017</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -538,22 +539,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.8365885416666666</v>
+        <v>0.8348958333333333</v>
       </c>
       <c r="C7">
-        <v>0.9180964638669445</v>
+        <v>0.9158589165885606</v>
       </c>
       <c r="D7">
-        <v>0.7818978459646002</v>
+        <v>0.7809402427834973</v>
       </c>
       <c r="E7">
-        <v>0.9338541666666667</v>
+        <v>0.9317708333333333</v>
       </c>
       <c r="F7">
-        <v>0.7818978459646002</v>
+        <v>0.7809402427834973</v>
       </c>
       <c r="G7">
-        <v>0.8510779640670165</v>
+        <v>0.8495253283407724</v>
       </c>
     </row>
   </sheetData>
@@ -594,22 +595,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8486979166666667</v>
+        <v>0.85078125</v>
       </c>
       <c r="C2">
-        <v>0.8909502909226364</v>
+        <v>0.8899047454384987</v>
       </c>
       <c r="D2">
-        <v>0.8160051465488265</v>
+        <v>0.8214462830222615</v>
       </c>
       <c r="E2">
-        <v>0.9020833333333333</v>
+        <v>0.8994791666666667</v>
       </c>
       <c r="F2">
-        <v>0.8160051465488265</v>
+        <v>0.8214462830222615</v>
       </c>
       <c r="G2">
-        <v>0.8564827072627742</v>
+        <v>0.8579073260141875</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -617,22 +618,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.962890625</v>
+        <v>0.96953125</v>
       </c>
       <c r="C3">
-        <v>0.9863747335304878</v>
+        <v>0.9866226778404528</v>
       </c>
       <c r="D3">
-        <v>0.9419154610575367</v>
+        <v>0.9540059264886415</v>
       </c>
       <c r="E3">
         <v>0.9869791666666666</v>
       </c>
       <c r="F3">
-        <v>0.9419154610575367</v>
+        <v>0.9540059264886415</v>
       </c>
       <c r="G3">
-        <v>0.9638307575340225</v>
+        <v>0.970108220629583</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -640,22 +641,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.8641927083333333</v>
+        <v>0.8729166666666667</v>
       </c>
       <c r="C4">
-        <v>0.965610764857632</v>
+        <v>0.9678422940670781</v>
       </c>
       <c r="D4">
-        <v>0.7996351929402803</v>
+        <v>0.8116010939347308</v>
       </c>
       <c r="E4">
-        <v>0.9731770833333333</v>
+        <v>0.9739583333333334</v>
       </c>
       <c r="F4">
-        <v>0.7996351929402803</v>
+        <v>0.8116010939347308</v>
       </c>
       <c r="G4">
-        <v>0.8777460325789996</v>
+        <v>0.884953766421864</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -663,22 +664,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.8643229166666667</v>
+        <v>0.865625</v>
       </c>
       <c r="C5">
-        <v>0.927594240709679</v>
+        <v>0.933628230533488</v>
       </c>
       <c r="D5">
-        <v>0.8180202006249785</v>
+        <v>0.8180479111908884</v>
       </c>
       <c r="E5">
-        <v>0.9380208333333333</v>
+        <v>0.94375</v>
       </c>
       <c r="F5">
-        <v>0.8180202006249785</v>
+        <v>0.8180479111908884</v>
       </c>
       <c r="G5">
-        <v>0.8737285095368116</v>
+        <v>0.8758230140092156</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -686,22 +687,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.9595052083333333</v>
+        <v>0.9671875</v>
       </c>
       <c r="C6">
-        <v>0.9833602662545963</v>
+        <v>0.9854259227781834</v>
       </c>
       <c r="D6">
-        <v>0.9384330903609321</v>
+        <v>0.9506203236695991</v>
       </c>
       <c r="E6">
-        <v>0.9841145833333333</v>
+        <v>0.9859375</v>
       </c>
       <c r="F6">
-        <v>0.9384330903609321</v>
+        <v>0.9506203236695991</v>
       </c>
       <c r="G6">
-        <v>0.9605903609930236</v>
+        <v>0.9678662161876035</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -709,22 +710,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.849609375</v>
+        <v>0.8526041666666667</v>
       </c>
       <c r="C7">
-        <v>0.9324749107681435</v>
+        <v>0.9293606508088482</v>
       </c>
       <c r="D7">
-        <v>0.7941496780874308</v>
+        <v>0.8005391311694824</v>
       </c>
       <c r="E7">
-        <v>0.9453125</v>
+        <v>0.9411458333333333</v>
       </c>
       <c r="F7">
-        <v>0.7941496780874308</v>
+        <v>0.8005391311694824</v>
       </c>
       <c r="G7">
-        <v>0.8629392289768811</v>
+        <v>0.8647474916355496</v>
       </c>
     </row>
   </sheetData>
@@ -765,22 +766,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.5032552083333334</v>
+        <v>0.5010416666666667</v>
       </c>
       <c r="C2">
-        <v>0.5074223440244925</v>
+        <v>0.5020401497205079</v>
       </c>
       <c r="D2">
-        <v>0.5020493265337899</v>
+        <v>0.5007026800932429</v>
       </c>
       <c r="E2">
-        <v>0.73125</v>
+        <v>0.7208333333333333</v>
       </c>
       <c r="F2">
-        <v>0.5020493265337899</v>
+        <v>0.5007026800932429</v>
       </c>
       <c r="G2">
-        <v>0.5952438552653917</v>
+        <v>0.5907457510130715</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -788,22 +789,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.96484375</v>
+        <v>0.959375</v>
       </c>
       <c r="C3">
-        <v>0.9923371580387091</v>
+        <v>0.9912511499384221</v>
       </c>
       <c r="D3">
-        <v>0.9404364987803713</v>
+        <v>0.9318695247326225</v>
       </c>
       <c r="E3">
-        <v>0.9927083333333333</v>
+        <v>0.9916666666666667</v>
       </c>
       <c r="F3">
-        <v>0.9404364987803713</v>
+        <v>0.9318695247326225</v>
       </c>
       <c r="G3">
-        <v>0.9658194164592599</v>
+        <v>0.9607112127740762</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -811,22 +812,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.531640625</v>
+        <v>0.5411458333333333</v>
       </c>
       <c r="C4">
-        <v>0.6408137027797198</v>
+        <v>0.6981170622463193</v>
       </c>
       <c r="D4">
-        <v>0.5178570213167865</v>
+        <v>0.5230505005057841</v>
       </c>
       <c r="E4">
-        <v>0.9174479166666667</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="F4">
-        <v>0.5178570213167865</v>
+        <v>0.5230505005057841</v>
       </c>
       <c r="G4">
-        <v>0.661992230749017</v>
+        <v>0.6703386882164902</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -834,22 +835,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5296875</v>
+        <v>0.534375</v>
       </c>
       <c r="C5">
-        <v>0.5655911443071411</v>
+        <v>0.5765415166730162</v>
       </c>
       <c r="D5">
-        <v>0.5192166150145886</v>
+        <v>0.5223352010449822</v>
       </c>
       <c r="E5">
-        <v>0.7924479166666667</v>
+        <v>0.7973958333333333</v>
       </c>
       <c r="F5">
-        <v>0.5192166150145886</v>
+        <v>0.5223352010449822</v>
       </c>
       <c r="G5">
-        <v>0.6272395363316702</v>
+        <v>0.6309781514637163</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -857,22 +858,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.9638020833333333</v>
+        <v>0.9682291666666667</v>
       </c>
       <c r="C6">
-        <v>0.9925992162994969</v>
+        <v>0.9946113259294572</v>
       </c>
       <c r="D6">
-        <v>0.9383512176677969</v>
+        <v>0.9451248822817467</v>
       </c>
       <c r="E6">
-        <v>0.99296875</v>
+        <v>0.9947916666666666</v>
       </c>
       <c r="F6">
-        <v>0.9383512176677969</v>
+        <v>0.9451248822817467</v>
       </c>
       <c r="G6">
-        <v>0.9648447343300357</v>
+        <v>0.969166687676167</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -880,22 +881,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5083333333333333</v>
+        <v>0.4997395833333333</v>
       </c>
       <c r="C7">
-        <v>0.5238775947310553</v>
+        <v>0.4999098482288729</v>
       </c>
       <c r="D7">
-        <v>0.5050577498125336</v>
+        <v>0.499815256527091</v>
       </c>
       <c r="E7">
-        <v>0.8268229166666666</v>
+        <v>0.8208333333333333</v>
       </c>
       <c r="F7">
-        <v>0.5050577498125336</v>
+        <v>0.499815256527091</v>
       </c>
       <c r="G7">
-        <v>0.6270236250216156</v>
+        <v>0.6211640040857177</v>
       </c>
     </row>
   </sheetData>
@@ -936,22 +937,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.5462239583333334</v>
+        <v>0.5489583333333333</v>
       </c>
       <c r="C2">
-        <v>0.588519415633979</v>
+        <v>0.5891536835158014</v>
       </c>
       <c r="D2">
-        <v>0.5313656522526329</v>
+        <v>0.5338912074759978</v>
       </c>
       <c r="E2">
-        <v>0.78359375</v>
+        <v>0.7890625</v>
       </c>
       <c r="F2">
-        <v>0.5313656522526329</v>
+        <v>0.5338912074759978</v>
       </c>
       <c r="G2">
-        <v>0.6331658115315447</v>
+        <v>0.6363516621066385</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -959,22 +960,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5604166666666667</v>
+        <v>0.5598958333333334</v>
       </c>
       <c r="C3">
-        <v>0.6229613316155068</v>
+        <v>0.619242440019829</v>
       </c>
       <c r="D3">
-        <v>0.5402853209341071</v>
+        <v>0.5403948433656248</v>
       </c>
       <c r="E3">
-        <v>0.8151041666666666</v>
+        <v>0.809375</v>
       </c>
       <c r="F3">
-        <v>0.5402853209341071</v>
+        <v>0.5403948433656248</v>
       </c>
       <c r="G3">
-        <v>0.6496142434753553</v>
+        <v>0.647712764775512</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -982,22 +983,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.512890625</v>
+        <v>0.5075520833333333</v>
       </c>
       <c r="C4">
-        <v>0.5375109428615992</v>
+        <v>0.5317490961442006</v>
       </c>
       <c r="D4">
-        <v>0.5077653820246886</v>
+        <v>0.5042950462172381</v>
       </c>
       <c r="E4">
-        <v>0.8546875</v>
+        <v>0.8463541666666666</v>
       </c>
       <c r="F4">
-        <v>0.5077653820246886</v>
+        <v>0.5042950462172381</v>
       </c>
       <c r="G4">
-        <v>0.6369279067105448</v>
+        <v>0.6317916588874618</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1005,22 +1006,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5403645833333334</v>
+        <v>0.53359375</v>
       </c>
       <c r="C5">
-        <v>0.5867597055318275</v>
+        <v>0.5714667078242347</v>
       </c>
       <c r="D5">
-        <v>0.5263929430920629</v>
+        <v>0.5221417460128234</v>
       </c>
       <c r="E5">
-        <v>0.80703125</v>
+        <v>0.7979166666666667</v>
       </c>
       <c r="F5">
-        <v>0.5263929430920629</v>
+        <v>0.5221417460128234</v>
       </c>
       <c r="G5">
-        <v>0.6370343828462777</v>
+        <v>0.6309355869408093</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1028,22 +1029,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.555078125</v>
+        <v>0.5559895833333334</v>
       </c>
       <c r="C6">
-        <v>0.6041459619291852</v>
+        <v>0.6099966214931587</v>
       </c>
       <c r="D6">
-        <v>0.53762219824375</v>
+        <v>0.5378592576596339</v>
       </c>
       <c r="E6">
-        <v>0.79296875</v>
+        <v>0.7947916666666667</v>
       </c>
       <c r="F6">
-        <v>0.53762219824375</v>
+        <v>0.5378592576596339</v>
       </c>
       <c r="G6">
-        <v>0.640567910986929</v>
+        <v>0.6412538169887511</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1051,22 +1052,193 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5430989583333333</v>
+        <v>0.540625</v>
       </c>
       <c r="C7">
-        <v>0.6289553581329125</v>
+        <v>0.6190579031213258</v>
       </c>
       <c r="D7">
-        <v>0.5259440260570946</v>
+        <v>0.5246495308745153</v>
       </c>
       <c r="E7">
-        <v>0.8763020833333334</v>
+        <v>0.8755208333333333</v>
       </c>
       <c r="F7">
-        <v>0.5259440260570946</v>
+        <v>0.5246495308745153</v>
       </c>
       <c r="G7">
-        <v>0.6572849086374037</v>
+        <v>0.655960186406647</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.5526041666666667</v>
+      </c>
+      <c r="C2">
+        <v>0.6549639690325181</v>
+      </c>
+      <c r="D2">
+        <v>0.5317837525038128</v>
+      </c>
+      <c r="E2">
+        <v>0.8921875</v>
+      </c>
+      <c r="F2">
+        <v>0.5317837525038128</v>
+      </c>
+      <c r="G2">
+        <v>0.6662450133159682</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.5653645833333333</v>
+      </c>
+      <c r="C3">
+        <v>0.6671130619485622</v>
+      </c>
+      <c r="D3">
+        <v>0.5410074393019572</v>
+      </c>
+      <c r="E3">
+        <v>0.8744791666666667</v>
+      </c>
+      <c r="F3">
+        <v>0.5410074393019572</v>
+      </c>
+      <c r="G3">
+        <v>0.6681982559939662</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.54296875</v>
+      </c>
+      <c r="C4">
+        <v>0.7535540385540387</v>
+      </c>
+      <c r="D4">
+        <v>0.5235627476027453</v>
+      </c>
+      <c r="E4">
+        <v>0.9604166666666667</v>
+      </c>
+      <c r="F4">
+        <v>0.5235627476027453</v>
+      </c>
+      <c r="G4">
+        <v>0.6776363306495852</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.55859375</v>
+      </c>
+      <c r="C5">
+        <v>0.8420996133496134</v>
+      </c>
+      <c r="D5">
+        <v>0.5322199886836917</v>
+      </c>
+      <c r="E5">
+        <v>0.9729166666666667</v>
+      </c>
+      <c r="F5">
+        <v>0.5322199886836917</v>
+      </c>
+      <c r="G5">
+        <v>0.6879816891958406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.55859375</v>
+      </c>
+      <c r="C6">
+        <v>0.6611588083908793</v>
+      </c>
+      <c r="D6">
+        <v>0.5360671837765901</v>
+      </c>
+      <c r="E6">
+        <v>0.8786458333333333</v>
+      </c>
+      <c r="F6">
+        <v>0.5360671837765901</v>
+      </c>
+      <c r="G6">
+        <v>0.6656759121339679</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.4971354166666667</v>
+      </c>
+      <c r="C7">
+        <v>0.4852966795783796</v>
+      </c>
+      <c r="D7">
+        <v>0.4984546480210013</v>
+      </c>
+      <c r="E7">
+        <v>0.8536458333333333</v>
+      </c>
+      <c r="F7">
+        <v>0.4984546480210013</v>
+      </c>
+      <c r="G7">
+        <v>0.6293188090104486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>